<commit_message>
Màj Journal de bord
Tout est dans le titre
</commit_message>
<xml_diff>
--- a/BLAColoc/Documentation/Journal de bord.xlsx
+++ b/BLAColoc/Documentation/Journal de bord.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian.RODRIGUES-FRAG\OneDrive - CPNV\GitHub\Projet_Web_ALB\BLAColoc\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Second year\Projet Web\Projet_Web_ALB\Projet_Web_ALB\Projet_Web_ALB\BLAColoc\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715"/>
   </bookViews>
   <sheets>
     <sheet name="Alexandre" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>DATE</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>Création d'un logo</t>
+  </si>
+  <si>
+    <t>création d'une ébauche JSON</t>
   </si>
 </sst>
 </file>
@@ -310,8 +313,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Log" displayName="Log" ref="B2:C7" totalsRowShown="0">
-  <autoFilter ref="B2:C7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Log" displayName="Log" ref="B2:C8" totalsRowShown="0">
+  <autoFilter ref="B2:C8"/>
   <tableColumns count="2">
     <tableColumn id="1" name="DATE" dataCellStyle="Date Column"/>
     <tableColumn id="3" name="ÉVÉNEMENT" dataCellStyle="Event Column"/>
@@ -587,10 +590,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:C7"/>
+  <dimension ref="B1:C8"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -652,6 +655,14 @@
       </c>
       <c r="C7" s="5" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>43158</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -680,7 +691,7 @@
   </sheetPr>
   <dimension ref="B1:C10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -880,6 +891,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <VSO_x0020_item_x0020_id xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Assetid_x0020_ xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Item_x0020_Details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Template_x0020_details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA3F7D94069FF64A86F7DFF56D60E3BE" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c32302c77d4085ecf495bdddb7f5e889">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a4f35948-e619-41b3-aa29-22878b09cfd2" xmlns:ns3="40262f94-9f35-4ac3-9a90-690165a166b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ab5ae46be95f9d0be6107e8200be7a2" ns2:_="" ns3:_="">
     <xsd:import namespace="a4f35948-e619-41b3-aa29-22878b09cfd2"/>
@@ -1060,27 +1091,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <VSO_x0020_item_x0020_id xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Assetid_x0020_ xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Item_x0020_Details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Template_x0020_details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1934E82E-1C0E-415F-9886-064BC72C3B49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{885137DC-D143-4691-87B9-2812AFF1A34F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="40262f94-9f35-4ac3-9a90-690165a166b7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B53890C6-895E-4346-BCB4-738C50EDC5D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1097,22 +1126,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{885137DC-D143-4691-87B9-2812AFF1A34F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="40262f94-9f35-4ac3-9a90-690165a166b7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1934E82E-1C0E-415F-9886-064BC72C3B49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Correction de la structure des dossiers
</commit_message>
<xml_diff>
--- a/BLAColoc/Documentation/Journal de bord.xlsx
+++ b/BLAColoc/Documentation/Journal de bord.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Second year\Projet Web\Projet_Web_ALB\Projet_Web_ALB\Projet_Web_ALB\BLAColoc\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian.RODRIGUES-FRAG\OneDrive - CPNV\GitHub\Projet_Web_ALB\BLAColoc\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Alexandre" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>DATE</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Modification du site, renommage des menus et supression de la base de donéée de base, création de vue et adaptation du contrôleur</t>
+  </si>
+  <si>
+    <t>Mise en place du serveur Web</t>
   </si>
 </sst>
 </file>
@@ -341,8 +344,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Log_5" displayName="Log_5" ref="B2:C10" totalsRowShown="0">
-  <autoFilter ref="B2:C10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Log_5" displayName="Log_5" ref="B2:C11" totalsRowShown="0">
+  <autoFilter ref="B2:C11"/>
   <tableColumns count="2">
     <tableColumn id="1" name="DATE" dataCellStyle="Date Column"/>
     <tableColumn id="3" name="ÉVÉNEMENT" dataCellStyle="Event Column"/>
@@ -604,7 +607,7 @@
   </sheetPr>
   <dimension ref="B1:C12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -733,10 +736,10 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:C10"/>
+  <dimension ref="B1:C11"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -822,6 +825,14 @@
       </c>
       <c r="C10" s="5" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
+        <v>43172</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -944,17 +955,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <VSO_x0020_item_x0020_id xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Assetid_x0020_ xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Item_x0020_Details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Template_x0020_details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA3F7D94069FF64A86F7DFF56D60E3BE" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c32302c77d4085ecf495bdddb7f5e889">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a4f35948-e619-41b3-aa29-22878b09cfd2" xmlns:ns3="40262f94-9f35-4ac3-9a90-690165a166b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ab5ae46be95f9d0be6107e8200be7a2" ns2:_="" ns3:_="">
     <xsd:import namespace="a4f35948-e619-41b3-aa29-22878b09cfd2"/>
@@ -1135,6 +1135,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <VSO_x0020_item_x0020_id xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Assetid_x0020_ xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Item_x0020_Details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Template_x0020_details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1934E82E-1C0E-415F-9886-064BC72C3B49}">
   <ds:schemaRefs>
@@ -1144,16 +1155,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{885137DC-D143-4691-87B9-2812AFF1A34F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="40262f94-9f35-4ac3-9a90-690165a166b7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B53890C6-895E-4346-BCB4-738C50EDC5D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1170,4 +1171,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{885137DC-D143-4691-87B9-2812AFF1A34F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="40262f94-9f35-4ac3-9a90-690165a166b7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Contacts et vue apparts
Modification de la taille du champs de contacts et ébauche de la vue des détails des apparts
</commit_message>
<xml_diff>
--- a/BLAColoc/Documentation/Journal de bord.xlsx
+++ b/BLAColoc/Documentation/Journal de bord.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Second year\Projet Web\Projet_Web_ALB\Projet_Web_ALB\Projet_Web_ALB\BLAColoc\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Projet Web\Projet_Web_ALB\BLAColoc\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11712"/>
   </bookViews>
   <sheets>
     <sheet name="Alexandre" sheetId="1" r:id="rId1"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
@@ -610,24 +610,24 @@
   </sheetPr>
   <dimension ref="B1:C13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" customWidth="1"/>
-    <col min="3" max="3" width="121.42578125" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="2" max="2" width="28.88671875" customWidth="1"/>
+    <col min="3" max="3" width="121.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" s="1" customFormat="1" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:3" s="1" customFormat="1" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C1"/>
     </row>
-    <row r="2" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -635,7 +635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2">
         <v>43140</v>
       </c>
@@ -643,7 +643,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <v>43143</v>
       </c>
@@ -651,7 +651,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <v>43143</v>
       </c>
@@ -659,7 +659,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <v>43144</v>
       </c>
@@ -667,7 +667,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <v>43144</v>
       </c>
@@ -675,7 +675,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>43158</v>
       </c>
@@ -683,7 +683,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <v>43164</v>
       </c>
@@ -691,7 +691,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2">
         <v>43165</v>
       </c>
@@ -699,7 +699,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <v>43167</v>
       </c>
@@ -707,7 +707,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2">
         <v>43172</v>
       </c>
@@ -715,7 +715,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2">
         <v>43174</v>
       </c>
@@ -753,20 +753,20 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" customWidth="1"/>
-    <col min="3" max="3" width="121.42578125" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="2" max="2" width="28.88671875" customWidth="1"/>
+    <col min="3" max="3" width="121.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" s="1" customFormat="1" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:3" s="1" customFormat="1" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C1"/>
     </row>
-    <row r="2" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -774,7 +774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2">
         <v>43132</v>
       </c>
@@ -782,7 +782,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <v>43136</v>
       </c>
@@ -790,7 +790,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <v>43137</v>
       </c>
@@ -798,7 +798,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <v>43140</v>
       </c>
@@ -806,7 +806,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <v>43143</v>
       </c>
@@ -814,7 +814,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>43143</v>
       </c>
@@ -822,7 +822,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <v>43144</v>
       </c>
@@ -830,7 +830,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2">
         <v>43144</v>
       </c>
@@ -838,7 +838,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <v>43172</v>
       </c>
@@ -876,20 +876,20 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" customWidth="1"/>
-    <col min="3" max="3" width="121.42578125" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="2" max="2" width="28.88671875" customWidth="1"/>
+    <col min="3" max="3" width="121.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" s="1" customFormat="1" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:3" s="1" customFormat="1" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C1"/>
     </row>
-    <row r="2" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -897,7 +897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2">
         <v>43141</v>
       </c>
@@ -905,7 +905,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <v>43137</v>
       </c>
@@ -913,7 +913,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <v>43140</v>
       </c>
@@ -921,7 +921,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <v>43143</v>
       </c>
@@ -929,7 +929,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <v>43144</v>
       </c>
@@ -968,6 +968,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA3F7D94069FF64A86F7DFF56D60E3BE" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c32302c77d4085ecf495bdddb7f5e889">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a4f35948-e619-41b3-aa29-22878b09cfd2" xmlns:ns3="40262f94-9f35-4ac3-9a90-690165a166b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ab5ae46be95f9d0be6107e8200be7a2" ns2:_="" ns3:_="">
     <xsd:import namespace="a4f35948-e619-41b3-aa29-22878b09cfd2"/>
@@ -1148,15 +1157,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{885137DC-D143-4691-87B9-2812AFF1A34F}">
   <ds:schemaRefs>
@@ -1168,6 +1168,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1934E82E-1C0E-415F-9886-064BC72C3B49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B53890C6-895E-4346-BCB4-738C50EDC5D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1184,12 +1192,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1934E82E-1C0E-415F-9886-064BC72C3B49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>